<commit_message>
Update spelling and add new graph and add start of chagne at election
</commit_message>
<xml_diff>
--- a/inputs/misc/misc_elections_data.xlsx
+++ b/inputs/misc/misc_elections_data.xlsx
@@ -5,23 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanalexander/Documents/phd/hansard/data/misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanalexander/Documents/phd/hansard/inputs/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30951456-8282-6C47-9D48-08E398B14AC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FD5EC1-AF00-5342-B682-B20A953AAAD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30820" yWindow="-10340" windowWidth="22920" windowHeight="23560" xr2:uid="{BF753662-51A7-C348-9337-8D82CA069EB9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22920" windowHeight="17540" xr2:uid="{BF753662-51A7-C348-9337-8D82CA069EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$121</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,132 +44,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>13 April 1910</t>
-  </si>
-  <si>
-    <t>31 May 1913</t>
-  </si>
-  <si>
-    <t>5 September 1914</t>
-  </si>
-  <si>
-    <t>5 May 1917</t>
-  </si>
-  <si>
-    <t>13 December 1919</t>
-  </si>
-  <si>
-    <t>16 December 1922</t>
-  </si>
-  <si>
-    <t>14 November 1925</t>
-  </si>
-  <si>
-    <t>17 November 1928</t>
-  </si>
-  <si>
-    <t>12 October 1929</t>
-  </si>
-  <si>
-    <t>19 December 1931</t>
-  </si>
-  <si>
-    <t>15 September 1934</t>
-  </si>
-  <si>
-    <t>23 October 1937</t>
-  </si>
-  <si>
-    <t>21 September 1940</t>
-  </si>
-  <si>
-    <t>21 August 1943</t>
-  </si>
-  <si>
-    <t>28 September 1946</t>
-  </si>
-  <si>
-    <t>10 December 1949</t>
-  </si>
-  <si>
-    <t>28 April 1951</t>
-  </si>
-  <si>
-    <t>29 May 1954</t>
-  </si>
-  <si>
-    <t>10 December 1955</t>
-  </si>
-  <si>
-    <t>22 November 1958</t>
-  </si>
-  <si>
-    <t>9 December 1961</t>
-  </si>
-  <si>
-    <t>30 November 1963</t>
-  </si>
-  <si>
-    <t>26 November 1966</t>
-  </si>
-  <si>
-    <t>25 October 1969</t>
-  </si>
-  <si>
-    <t>2 December 1972</t>
-  </si>
-  <si>
-    <t>18 May 1974</t>
-  </si>
-  <si>
-    <t>13 December 1975</t>
-  </si>
-  <si>
-    <t>10 December 1977</t>
-  </si>
-  <si>
-    <t>18 October 1980</t>
-  </si>
-  <si>
-    <t>5 March 1983</t>
-  </si>
-  <si>
-    <t>1 December 1984</t>
-  </si>
-  <si>
-    <t>11 July 1987</t>
-  </si>
-  <si>
-    <t>24 March 1990</t>
-  </si>
-  <si>
-    <t>13 March 1993</t>
-  </si>
-  <si>
-    <t>2 March 1996</t>
-  </si>
-  <si>
-    <t>3 October 1998</t>
-  </si>
-  <si>
-    <t>10 November 2001</t>
-  </si>
-  <si>
-    <t>9 October 2004</t>
-  </si>
-  <si>
-    <t>24 November 2007</t>
-  </si>
-  <si>
-    <t>21 August 2010</t>
-  </si>
-  <si>
-    <t>7 September 2013</t>
-  </si>
-  <si>
-    <t>2 July 2016</t>
-  </si>
-  <si>
     <t>Non-labor</t>
   </si>
   <si>
@@ -198,15 +77,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>29 March 1901</t>
-  </si>
-  <si>
-    <t>16 December 1903</t>
-  </si>
-  <si>
-    <t>12 December 1906</t>
-  </si>
-  <si>
     <t>Curtin '43</t>
   </si>
   <si>
@@ -229,6 +99,141 @@
   </si>
   <si>
     <t>First election</t>
+  </si>
+  <si>
+    <t>1901-03-29</t>
+  </si>
+  <si>
+    <t>1903-12-16</t>
+  </si>
+  <si>
+    <t>1906-12-12</t>
+  </si>
+  <si>
+    <t>1910-04-13</t>
+  </si>
+  <si>
+    <t>1913-05-31</t>
+  </si>
+  <si>
+    <t>1914-09-05</t>
+  </si>
+  <si>
+    <t>1917-05-05</t>
+  </si>
+  <si>
+    <t>1919-12-13</t>
+  </si>
+  <si>
+    <t>1922-12-16</t>
+  </si>
+  <si>
+    <t>1925-11-14</t>
+  </si>
+  <si>
+    <t>1928-11-17</t>
+  </si>
+  <si>
+    <t>1929-10-12</t>
+  </si>
+  <si>
+    <t>1931-12-19</t>
+  </si>
+  <si>
+    <t>1934-09-15</t>
+  </si>
+  <si>
+    <t>1937-10-23</t>
+  </si>
+  <si>
+    <t>1940-09-21</t>
+  </si>
+  <si>
+    <t>1943-08-21</t>
+  </si>
+  <si>
+    <t>1946-09-28</t>
+  </si>
+  <si>
+    <t>1949-12-10</t>
+  </si>
+  <si>
+    <t>1951-08-28</t>
+  </si>
+  <si>
+    <t>1954-05-29</t>
+  </si>
+  <si>
+    <t>1955-12-10</t>
+  </si>
+  <si>
+    <t>1958-11-22</t>
+  </si>
+  <si>
+    <t>1961-12-09</t>
+  </si>
+  <si>
+    <t>1963-11-30</t>
+  </si>
+  <si>
+    <t>1966-11-26</t>
+  </si>
+  <si>
+    <t>1969-10-25</t>
+  </si>
+  <si>
+    <t>1972-12-02</t>
+  </si>
+  <si>
+    <t>1974-05-18</t>
+  </si>
+  <si>
+    <t>1975-12-13</t>
+  </si>
+  <si>
+    <t>1977-12-10</t>
+  </si>
+  <si>
+    <t>1980-10-18</t>
+  </si>
+  <si>
+    <t>1983-03-05</t>
+  </si>
+  <si>
+    <t>1984-12-01</t>
+  </si>
+  <si>
+    <t>1987-07-11</t>
+  </si>
+  <si>
+    <t>1990-03-24</t>
+  </si>
+  <si>
+    <t>1993-03-13</t>
+  </si>
+  <si>
+    <t>1996-03-02</t>
+  </si>
+  <si>
+    <t>1998-10-03</t>
+  </si>
+  <si>
+    <t>2001-11-10</t>
+  </si>
+  <si>
+    <t>2004-10-09</t>
+  </si>
+  <si>
+    <t>2007-11-24</t>
+  </si>
+  <si>
+    <t>2010-08-21</t>
+  </si>
+  <si>
+    <t>2013-09-07</t>
+  </si>
+  <si>
+    <t>2016-07-02</t>
   </si>
 </sst>
 </file>
@@ -264,9 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,12 +590,12 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1"/>
   </cols>
@@ -605,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -621,17 +627,17 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>56</v>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D2">
         <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -646,14 +652,14 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>57</v>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D4">
         <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -673,14 +679,14 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>58</v>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D7">
         <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -705,14 +711,14 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D11">
         <v>75</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -732,14 +738,14 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D14">
         <v>75</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -749,17 +755,17 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D15">
         <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -779,14 +785,14 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
+      <c r="C18" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D18">
         <v>75</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -801,17 +807,17 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D20">
         <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -831,14 +837,14 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>8</v>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D23">
         <v>75</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -858,14 +864,14 @@
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D26">
         <v>75</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -885,14 +891,14 @@
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>10</v>
+      <c r="C29" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D29">
         <v>75</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -902,17 +908,17 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
+      <c r="C30" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D30">
         <v>75</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -927,17 +933,17 @@
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>12</v>
+      <c r="C32" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D32">
         <v>75</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -957,17 +963,17 @@
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>13</v>
+      <c r="C35" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D35">
         <v>74</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -987,14 +993,14 @@
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>14</v>
+      <c r="C38" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D38">
         <v>74</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1014,14 +1020,14 @@
       <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>15</v>
+      <c r="C41" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D41">
         <v>74</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1041,17 +1047,17 @@
       <c r="B44">
         <v>1</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>16</v>
+      <c r="C44" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D44">
         <v>74</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1071,14 +1077,14 @@
       <c r="B47">
         <v>1</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>17</v>
+      <c r="C47" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="D47">
         <v>74</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1098,17 +1104,17 @@
       <c r="B50">
         <v>1</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>18</v>
+      <c r="C50" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D50">
         <v>121</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1123,17 +1129,17 @@
       <c r="B52">
         <v>1</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>19</v>
+      <c r="C52" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D52">
         <v>121</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1153,14 +1159,14 @@
       <c r="B55">
         <v>1</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>20</v>
+      <c r="C55" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D55">
         <v>121</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1170,17 +1176,17 @@
       <c r="B56">
         <v>1</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>21</v>
+      <c r="C56" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D56">
         <v>122</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1200,14 +1206,14 @@
       <c r="B59">
         <v>1</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>22</v>
+      <c r="C59" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D59">
         <v>122</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1227,14 +1233,14 @@
       <c r="B62">
         <v>1</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>23</v>
+      <c r="C62" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D62">
         <v>122</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1249,14 +1255,14 @@
       <c r="B64">
         <v>1</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>24</v>
+      <c r="C64" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="D64">
         <v>122</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1276,14 +1282,14 @@
       <c r="B67">
         <v>1</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>25</v>
+      <c r="C67" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D67">
         <v>124</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1303,14 +1309,14 @@
       <c r="B70">
         <v>1</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>26</v>
+      <c r="C70" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D70">
         <v>125</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1330,14 +1336,14 @@
       <c r="B73">
         <v>1</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>27</v>
+      <c r="C73" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D73">
         <v>125</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1352,14 +1358,14 @@
       <c r="B75">
         <v>1</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>28</v>
+      <c r="C75" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D75">
         <v>127</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1369,17 +1375,17 @@
       <c r="B76">
         <v>1</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>29</v>
+      <c r="C76" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D76">
         <v>127</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1394,14 +1400,14 @@
       <c r="B78">
         <v>1</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>30</v>
+      <c r="C78" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D78">
         <v>124</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1421,14 +1427,14 @@
       <c r="B81">
         <v>1</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>31</v>
+      <c r="C81" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D81">
         <v>125</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1448,14 +1454,14 @@
       <c r="B84">
         <v>1</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>32</v>
+      <c r="C84" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D84">
         <v>125</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1465,14 +1471,14 @@
       <c r="B85">
         <v>1</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>33</v>
+      <c r="C85" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D85">
         <v>148</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -1492,17 +1498,17 @@
       <c r="B88">
         <v>1</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>34</v>
+      <c r="C88" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D88">
         <v>148</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -1522,14 +1528,14 @@
       <c r="B91">
         <v>1</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>35</v>
+      <c r="C91" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D91">
         <v>148</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -1549,14 +1555,14 @@
       <c r="B94">
         <v>1</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>36</v>
+      <c r="C94" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D94">
         <v>147</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -1576,17 +1582,17 @@
       <c r="B97">
         <v>1</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>37</v>
+      <c r="C97" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D97">
         <v>148</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -1601,14 +1607,14 @@
       <c r="B99">
         <v>1</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>38</v>
+      <c r="C99" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D99">
         <v>148</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -1628,14 +1634,14 @@
       <c r="B102">
         <v>1</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>39</v>
+      <c r="C102" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D102">
         <v>150</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -1655,14 +1661,14 @@
       <c r="B105">
         <v>1</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>40</v>
+      <c r="C105" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D105">
         <v>150</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -1682,17 +1688,17 @@
       <c r="B108">
         <v>1</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>41</v>
+      <c r="C108" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D108">
         <v>150</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -1712,14 +1718,14 @@
       <c r="B111">
         <v>1</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>42</v>
+      <c r="C111" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D111">
         <v>150</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -1739,14 +1745,14 @@
       <c r="B114">
         <v>1</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>43</v>
+      <c r="C114" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D114">
         <v>150</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1766,14 +1772,14 @@
       <c r="B117">
         <v>1</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>44</v>
+      <c r="C117" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D117">
         <v>150</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -1797,7 +1803,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C124" xr:uid="{D8A78FBE-F9BA-2B40-9CE4-2237253FCFE1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>